<commit_message>
updated data extraction file
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_VanHoey.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_VanHoey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457EDC4F-FF76-43DF-864D-CBECF31EC4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615E13AE-7E37-4FCB-9369-84860EF145A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCall" sheetId="1" r:id="rId1"/>
@@ -2388,7 +2388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3081" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3098" uniqueCount="711">
   <si>
     <t>SearchID</t>
   </si>
@@ -5895,10 +5895,10 @@
   <dimension ref="A1:AZ120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AJ24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AV18" sqref="AV18"/>
+      <selection pane="bottomRight" activeCell="AQ29" sqref="AQ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5"/>
@@ -8896,7 +8896,10 @@
         <v>686</v>
       </c>
       <c r="AN24" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO24" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP24" s="21" t="s">
         <v>571</v>
@@ -9027,7 +9030,10 @@
         <v>686</v>
       </c>
       <c r="AN25" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO25" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP25" s="21" t="s">
         <v>571</v>
@@ -9158,7 +9164,10 @@
         <v>686</v>
       </c>
       <c r="AN26" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO26" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP26" s="21" t="s">
         <v>571</v>
@@ -9289,7 +9298,10 @@
         <v>686</v>
       </c>
       <c r="AN27" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO27" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP27" s="21" t="s">
         <v>571</v>
@@ -9417,7 +9429,10 @@
         <v>534</v>
       </c>
       <c r="AN28" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO28" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP28" s="21" t="s">
         <v>571</v>
@@ -9548,7 +9563,10 @@
         <v>534</v>
       </c>
       <c r="AN29" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO29" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP29" s="21" t="s">
         <v>571</v>
@@ -9679,7 +9697,10 @@
         <v>534</v>
       </c>
       <c r="AN30" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO30" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP30" s="21" t="s">
         <v>571</v>
@@ -9807,7 +9828,10 @@
         <v>687</v>
       </c>
       <c r="AN31" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO31" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP31" s="21" t="s">
         <v>571</v>
@@ -9938,7 +9962,10 @@
         <v>687</v>
       </c>
       <c r="AN32" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO32" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP32" s="21" t="s">
         <v>571</v>
@@ -10069,7 +10096,10 @@
         <v>687</v>
       </c>
       <c r="AN33" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO33" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP33" s="21" t="s">
         <v>571</v>
@@ -10197,7 +10227,10 @@
         <v>688</v>
       </c>
       <c r="AN34" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO34" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP34" s="21" t="s">
         <v>571</v>
@@ -10328,7 +10361,10 @@
         <v>688</v>
       </c>
       <c r="AN35" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO35" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP35" s="21" t="s">
         <v>571</v>
@@ -10459,7 +10495,10 @@
         <v>688</v>
       </c>
       <c r="AN36" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO36" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP36" s="21" t="s">
         <v>571</v>
@@ -10587,7 +10626,10 @@
         <v>689</v>
       </c>
       <c r="AN37" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO37" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP37" s="21" t="s">
         <v>571</v>
@@ -10718,7 +10760,10 @@
         <v>689</v>
       </c>
       <c r="AN38" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO38" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP38" s="21" t="s">
         <v>571</v>
@@ -10846,7 +10891,10 @@
         <v>690</v>
       </c>
       <c r="AN39" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO39" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP39" s="21" t="s">
         <v>571</v>
@@ -10974,7 +11022,10 @@
         <v>690</v>
       </c>
       <c r="AN40" s="21" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AO40" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="AP40" s="21" t="s">
         <v>571</v>
@@ -15669,7 +15720,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR3:AR1048576" xr:uid="{5FFD7ACF-9A7A-47E4-8F02-C092CA18B67C}">
       <formula1>Fishery_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS3:AT1048576 AO3:AO1048576 AJ3:AK1048576" xr:uid="{E3465DE4-B915-4C62-9316-EABEC40DC1E6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS3:AT1048576 AJ3:AK1048576 AO3:AO1048576" xr:uid="{E3465DE4-B915-4C62-9316-EABEC40DC1E6}">
       <formula1>INDIRECT(AI3)</formula1>
     </dataValidation>
   </dataValidations>
@@ -17773,6 +17824,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abe771af6212f3f785694fa6f4ad1686">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -17886,31 +17946,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{296C6747-B437-4BFD-90D3-AF1F913D3FA0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17924,12 +17983,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>